<commit_message>
Modifying a basic example
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -12,9 +12,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>This is cell A1</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Jaime</t>
+  </si>
+  <si>
+    <t>Cra 16 #115</t>
+  </si>
+  <si>
+    <t>Javier</t>
+  </si>
+  <si>
+    <t>Cra 14 #74-32</t>
+  </si>
+  <si>
+    <t>Eliana</t>
+  </si>
+  <si>
+    <t>Cra 7 #80</t>
   </si>
 </sst>
 </file>
@@ -58,9 +85,22 @@
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D4">
+  <autoFilter ref="A1:D4"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Name"/>
+    <tableColumn id="2" name="Id"/>
+    <tableColumn id="3" name="Address"/>
+    <tableColumn id="4" name="Age"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -70,8 +110,62 @@
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0">
+        <v>3242424</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="0">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="0">
+        <v>3242444</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="0">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="0">
+        <v>3246244</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="0">
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
   <headerFooter/>
+  <tableParts>
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>